<commit_message>
reorganized files. fixed forceStaircase.py
</commit_message>
<xml_diff>
--- a/JND_Study/JND_Data/2024-01-30_20-47.xlsx
+++ b/JND_Study/JND_Data/2024-01-30_20-47.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sreela/Documents/School/Stanford/Year3_2/PIEZO2/JND_Study/JND_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{684F924A-DC86-1647-A156-A27435E38873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE20FBA1-EBEA-6E45-ABE1-6B9A502508D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38480" yWindow="0" windowWidth="26740" windowHeight="22000" activeTab="1" xr2:uid="{1B4DE873-A15E-BD41-A0B0-8A0C0D8007DE}"/>
+    <workbookView xWindow="32900" yWindow="-2960" windowWidth="44060" windowHeight="25760" activeTab="1" xr2:uid="{1B4DE873-A15E-BD41-A0B0-8A0C0D8007DE}"/>
   </bookViews>
   <sheets>
     <sheet name="trial" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="forceOfStairCase_onePoke_2024_01_30_20_47" localSheetId="1">forceStaircase!$A$1:$F$51</definedName>
     <definedName name="trial_2024_01_30_20_47" localSheetId="0">trial!$A$1:$I$51</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +43,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{A1876DE3-0C14-534A-A8BD-7A0D28632357}" name="forceOfStairCase_onePoke_2024-01-30_20-47" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/Sreela/Documents/School/Stanford/Year3_2/PIEZO2/JND_Study/JND_Data/forceOfStairCase_onePoke_2024-01-30_20-47.csv" comma="1">
+    <textPr sourceFile="/Users/Sreela/Documents/School/Stanford/Year3_2/PIEZO2/JND_Study/JND_Data/forceOfStairCase_onePoke_2024-01-30_20-47.csv" comma="1">
       <textFields count="6">
         <textField/>
         <textField/>
@@ -55,7 +55,7 @@
     </textPr>
   </connection>
   <connection id="2" xr16:uid="{BC09CFE6-D28E-9E4E-B370-DFDD2A692B40}" name="trial_2024-01-30_20-47" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/Sreela/Documents/School/Stanford/Year3_2/PIEZO2/JND_Study/JND_Data/2024-01-30_20-47/trial_2024-01-30_20-47.csv" comma="1">
+    <textPr sourceFile="/Users/Sreela/Documents/School/Stanford/Year3_2/PIEZO2/JND_Study/JND_Data/2024-01-30_20-47/trial_2024-01-30_20-47.csv" comma="1">
       <textFields count="9">
         <textField/>
         <textField/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>trialCount</t>
   </si>
@@ -119,6 +119,12 @@
   <si>
     <t>stdevForce1</t>
   </si>
+  <si>
+    <t>12.32 + 0.55</t>
+  </si>
+  <si>
+    <t>10.72 + 0.55</t>
+  </si>
 </sst>
 </file>
 
@@ -140,12 +146,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -160,9 +172,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2246,7 +2259,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.9244874994831214E-2"/>
+          <c:y val="0.16624919927082912"/>
+          <c:w val="0.88958177353640089"/>
+          <c:h val="0.72976877235644666"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -5903,16 +5926,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>521741</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>51847</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>539750</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>141063</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>156542</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5939,15 +5962,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>482279</xdr:colOff>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>447164</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>109570</xdr:colOff>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>116520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6283,10 +6306,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{745143AA-55AE-3E40-8456-FB51B42ECA8A}">
-  <dimension ref="A1:S51"/>
+  <dimension ref="A1:Y51"/>
   <sheetViews>
-    <sheetView topLeftCell="J7" zoomScale="143" zoomScaleNormal="143" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8:S23"/>
+    <sheetView zoomScale="143" zoomScaleNormal="143" workbookViewId="0">
+      <selection activeCell="Y30" sqref="Y30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6829,7 +6852,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -6865,7 +6888,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -6901,7 +6924,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -6937,7 +6960,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -6973,7 +6996,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -7009,7 +7032,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -7044,8 +7067,23 @@
       <c r="S22">
         <v>101</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="U22">
+        <f>AVERAGE(S21:S23)</f>
+        <v>103.66666666666667</v>
+      </c>
+      <c r="V22" s="2">
+        <f>(U22-47)*20/(139-47)</f>
+        <v>12.318840579710146</v>
+      </c>
+      <c r="X22">
+        <v>96.33</v>
+      </c>
+      <c r="Y22" s="2">
+        <f>(X22-47)*20/(139-47)</f>
+        <v>10.723913043478261</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -7080,8 +7118,21 @@
       <c r="S23">
         <v>106</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="U23">
+        <f>STDEV(S21:S23)</f>
+        <v>2.5166114784235836</v>
+      </c>
+      <c r="V23" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="X23">
+        <v>2.52</v>
+      </c>
+      <c r="Y23" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -7110,7 +7161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -7138,8 +7189,14 @@
       <c r="I25">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="V25" t="s">
+        <v>15</v>
+      </c>
+      <c r="X25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -7168,7 +7225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -7197,7 +7254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -7226,7 +7283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -7255,7 +7312,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -7284,7 +7341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -7313,7 +7370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -7917,8 +7974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A85C539-6AFE-FB41-8E42-621377AD1F9A}">
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView tabSelected="1" topLeftCell="F2" zoomScale="197" zoomScaleNormal="197" workbookViewId="0">
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>